<commit_message>
show font awesome icons
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,6 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
@@ -148,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -251,15 +250,21 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="2" tint="-0.749992370372631"/>
-      <name val="Font Awesome 5 Free Regular"/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
+      <sz val="14"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Font Awesome 5 Free"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Font Awesome 5 Free"/>
     </font>
   </fonts>
   <fills count="15">
@@ -394,7 +399,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -423,18 +428,11 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -455,9 +453,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -469,6 +464,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1845,8 +1849,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1862,12 +1866,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
@@ -1929,10 +1933,10 @@
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
@@ -1955,7 +1959,7 @@
       <c r="B19" s="4">
         <v>6</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="25">
         <v>2400</v>
       </c>
       <c r="D19" s="6">
@@ -1970,7 +1974,7 @@
       <c r="B20" s="4">
         <v>3</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="25">
         <v>15</v>
       </c>
       <c r="D20" s="6">
@@ -1985,7 +1989,7 @@
       <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="25">
         <v>160</v>
       </c>
       <c r="D21" s="7">
@@ -2000,7 +2004,7 @@
       <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="25">
         <v>120</v>
       </c>
       <c r="D22" s="7">
@@ -2010,10 +2014,10 @@
     </row>
     <row r="23" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="25">
         <f>SUM(C19:C22)</f>
         <v>2695</v>
       </c>
@@ -2026,46 +2030,46 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34" t="s">
+      <c r="D25" s="30"/>
+      <c r="E25" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="9"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="9"/>
       <c r="J28" s="1"/>
     </row>
@@ -2091,8 +2095,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2103,23 +2107,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -2148,12 +2152,12 @@
       <c r="D4" s="19">
         <v>30</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="26">
         <f>C4*D4</f>
         <v>30</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
@@ -2162,12 +2166,12 @@
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -2176,10 +2180,10 @@
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
@@ -2188,39 +2192,39 @@
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="25"/>
+      <c r="B8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="26"/>
-      <c r="D9" s="37" t="s">
+      <c r="B9" s="23"/>
+      <c r="D9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="34" t="s">
+      <c r="E9" s="33"/>
+      <c r="F9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="38"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="16"/>

</xml_diff>

<commit_message>
implement logic to read cell value
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -444,6 +444,12 @@
     <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,6 +457,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -464,15 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1849,8 +1849,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:E28"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1866,12 +1866,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
@@ -1933,10 +1933,10 @@
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
@@ -2030,46 +2030,46 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="35" t="s">
+      <c r="D25" s="32"/>
+      <c r="E25" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="9"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
       <c r="I28" s="9"/>
       <c r="J28" s="1"/>
     </row>
@@ -2095,8 +2095,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2107,20 +2107,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
@@ -2167,7 +2167,7 @@
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="26"/>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="20"/>
@@ -2181,7 +2181,7 @@
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="36"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
     </row>
@@ -2193,38 +2193,38 @@
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="26"/>
-      <c r="F7" s="36"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23"/>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="35" t="s">
+      <c r="E9" s="36"/>
+      <c r="F9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="34"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="16"/>

</xml_diff>

<commit_message>
fix font awesome icon display problem
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Transportation</t>
   </si>
@@ -100,24 +100,6 @@
     <t>Done</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Font Awesome 5 Free Regular"/>
-      </rPr>
-      <t></t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Add your new expense </t>
-    </r>
-  </si>
-  <si>
     <t>Budget Expense Summary</t>
   </si>
   <si>
@@ -137,6 +119,9 @@
   </si>
   <si>
     <t>click to sum all expense by category and switch back to the previous sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Add your new expense </t>
   </si>
 </sst>
 </file>
@@ -236,11 +221,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Font Awesome 5 Free Regular"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
     </font>
@@ -264,6 +244,12 @@
       <b/>
       <sz val="24"/>
       <color theme="2" tint="-0.749992370372631"/>
+      <name val="Font Awesome 5 Free"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="Font Awesome 5 Free"/>
     </font>
   </fonts>
@@ -399,7 +385,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -426,8 +412,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -442,12 +428,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -459,20 +445,23 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -486,8 +475,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF4285F4"/>
       <color rgb="FFBDD7EE"/>
-      <color rgb="FF4285F4"/>
       <color rgb="FF6D9EEB"/>
       <color rgb="FF2FB5B6"/>
       <color rgb="FFFF7E79"/>
@@ -1850,7 +1839,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1867,7 +1856,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1943,7 +1932,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -2038,7 +2027,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
@@ -2096,7 +2085,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B7" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2107,24 +2096,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="A1" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>11</v>
@@ -2141,7 +2130,7 @@
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>0</v>
@@ -2161,23 +2150,19 @@
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="B5" s="18" t="s">
-        <v>0</v>
-      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="26"/>
       <c r="F5" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
-      <c r="B6" s="18" t="s">
-        <v>0</v>
-      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="26"/>
@@ -2187,9 +2172,7 @@
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
-      <c r="B7" s="18" t="s">
-        <v>0</v>
-      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="26"/>
@@ -2200,31 +2183,31 @@
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23"/>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="37"/>
+      <c r="G9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="33"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="16"/>

</xml_diff>

<commit_message>
* read specific rows of expense * minor change app.xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Transportation</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Taxi</t>
   </si>
   <si>
     <t> Add your new expense and choose corresponding category</t>
@@ -451,17 +448,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -760,16 +757,16 @@
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2400.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1889,7 +1886,7 @@
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <f>SUM(C19:C22)</f>
-        <v>2695</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1903,7 +1900,7 @@
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <f>A5-A8</f>
-        <v>305</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1932,7 +1929,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -1946,14 +1943,14 @@
         <v>0</v>
       </c>
       <c r="B19" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C19" s="25">
-        <v>2400</v>
-      </c>
-      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6" t="e">
         <f>C19/C23</f>
-        <v>0.89053803339517623</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -1961,14 +1958,14 @@
         <v>1</v>
       </c>
       <c r="B20" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="25">
-        <v>15</v>
-      </c>
-      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="e">
         <f>C20/C23</f>
-        <v>5.5658627087198514E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -1976,14 +1973,14 @@
         <v>2</v>
       </c>
       <c r="B21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C21" s="25">
-        <v>160</v>
-      </c>
-      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7" t="e">
         <f>C21/C23</f>
-        <v>5.9369202226345084E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -1991,14 +1988,14 @@
         <v>3</v>
       </c>
       <c r="B22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="25">
-        <v>120</v>
-      </c>
-      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="e">
         <f>C22/C23</f>
-        <v>4.4526901669758812E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -2008,11 +2005,11 @@
       </c>
       <c r="C23" s="25">
         <f>SUM(C19:C22)</f>
-        <v>2695</v>
-      </c>
-      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8" t="e">
         <f>SUM(D19:D22)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2027,7 +2024,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
@@ -2085,7 +2082,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B6:B7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2096,20 +2093,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="A1" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
@@ -2129,21 +2126,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19">
-        <v>1</v>
-      </c>
-      <c r="D4" s="19">
-        <v>30</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="26">
         <f>C4*D4</f>
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="20"/>
@@ -2153,9 +2145,9 @@
       <c r="B5" s="18"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="29" t="s">
-        <v>19</v>
+      <c r="E5" s="26">
+        <f t="shared" ref="E5:E7" si="0">C5*D5</f>
+        <v>0</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -2165,7 +2157,10 @@
       <c r="B6" s="18"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="26"/>
+      <c r="E6" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F6" s="28"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
@@ -2175,7 +2170,10 @@
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="26"/>
+      <c r="E7" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -2183,31 +2181,31 @@
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23"/>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="36"/>
+      <c r="G9" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="33"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="16"/>

</xml_diff>

<commit_message>
fix styles in app.xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -25,28 +25,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="C25" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>click to switch to the next sheet to add new expense</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -129,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -157,18 +135,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="2" tint="-0.499984740745262"/>
-      <name val="FZLanTingHei-M-GBK"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="2" tint="-0.499984740745262"/>
-      <name val="FZLanTingHei-M-GBK"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="24"/>
@@ -202,20 +168,10 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Font Awesome 5 Free Solid"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4285F4"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
@@ -225,17 +181,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="2" tint="-0.749992370372631"/>
-      <name val="Font Awesome 5 Free"/>
     </font>
     <font>
       <b/>
@@ -248,6 +193,28 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Font Awesome 5 Free"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4285F4"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Font Awesome 5 Free"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="FZLanTingHei-M-GBK"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="15">
@@ -385,79 +352,77 @@
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1829,14 +1794,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1852,12 +1817,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
@@ -1919,10 +1884,10 @@
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
@@ -1938,14 +1903,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="21">
         <v>0</v>
       </c>
       <c r="D19" s="6" t="e">
@@ -1953,14 +1918,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="4">
         <v>0</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="21">
         <v>0</v>
       </c>
       <c r="D20" s="6" t="e">
@@ -1968,14 +1933,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="21">
         <v>0</v>
       </c>
       <c r="D21" s="7" t="e">
@@ -1983,14 +1948,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="4">
         <v>0</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="21">
         <v>0</v>
       </c>
       <c r="D22" s="7" t="e">
@@ -1998,12 +1963,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="21">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
@@ -2016,46 +1981,46 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33" t="s">
+      <c r="D25" s="26"/>
+      <c r="E25" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="9"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="9"/>
       <c r="J28" s="1"/>
     </row>
@@ -2070,7 +2035,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2081,8 +2045,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2093,99 +2057,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="24" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="32" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="26">
+      <c r="A4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="22">
         <f>C4*D4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="26">
+      <c r="A5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="22">
         <f t="shared" ref="E5:E7" si="0">C5*D5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="26">
+      <c r="A6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="26">
+      <c r="A7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="22"/>
-    </row>
-    <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="23"/>
-      <c r="D9" s="37" t="s">
+      <c r="F7" s="34"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="33"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="33" t="s">
+      <c r="E9" s="36"/>
+      <c r="F9" s="37" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2193,17 +2172,23 @@
       </c>
       <c r="H9" s="38"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="33"/>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="33"/>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
     </row>
@@ -2217,9 +2202,15 @@
     <mergeCell ref="G9:H11"/>
     <mergeCell ref="F9:F11"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B7">
       <formula1>"Transportation, Lodging, Food, Entertainment"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C7">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D7">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update test excel file: replace font awesome icons with images
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Transportation</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Add my new expense</t>
-  </si>
-  <si>
-    <t></t>
   </si>
   <si>
     <t>Percentage</t>
@@ -84,19 +81,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t> Add your new expense and choose corresponding category</t>
-  </si>
-  <si>
     <t>No. of items</t>
   </si>
   <si>
-    <t>click to switch to the next sheet to add new expense</t>
-  </si>
-  <si>
-    <t>click to sum all expense by category and switch back to the previous sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Add your new expense </t>
+    <t xml:space="preserve">Add your new expense </t>
   </si>
 </sst>
 </file>
@@ -107,7 +95,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -135,11 +123,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color theme="2" tint="-0.499984740745262"/>
-      <name val="Font Awesome 5 Free Regular"/>
     </font>
     <font>
       <sz val="10"/>
@@ -183,18 +166,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="2" tint="-0.749992370372631"/>
-      <name val="Font Awesome 5 Free"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Font Awesome 5 Free"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF4285F4"/>
       <name val="Arial"/>
@@ -215,6 +186,20 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -349,81 +334,72 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1529,6 +1505,125 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5087938" y="5317861"/>
+          <a:ext cx="2563812" cy="427302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905500" y="469900"/>
+          <a:ext cx="2705100" cy="450850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>185775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905500" y="1689100"/>
+          <a:ext cx="2768600" cy="579475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1817,12 +1912,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
@@ -1832,7 +1927,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1845,7 +1940,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1859,7 +1954,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1884,23 +1979,23 @@
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -1910,7 +2005,7 @@
       <c r="B19" s="4">
         <v>0</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="20">
         <v>0</v>
       </c>
       <c r="D19" s="6" t="e">
@@ -1925,7 +2020,7 @@
       <c r="B20" s="4">
         <v>0</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <v>0</v>
       </c>
       <c r="D20" s="6" t="e">
@@ -1940,7 +2035,7 @@
       <c r="B21" s="4">
         <v>0</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>0</v>
       </c>
       <c r="D21" s="7" t="e">
@@ -1955,7 +2050,7 @@
       <c r="B22" s="4">
         <v>0</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>0</v>
       </c>
       <c r="D22" s="7" t="e">
@@ -1965,10 +2060,10 @@
     </row>
     <row r="23" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
@@ -1981,33 +2076,29 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="33"/>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
       <c r="H26" s="33"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="33"/>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
       <c r="H27" s="33"/>
@@ -2015,9 +2106,9 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="G28" s="33"/>
       <c r="H28" s="33"/>
@@ -2025,12 +2116,11 @@
       <c r="J28" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="C25:D28"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="F25:H28"/>
+    <mergeCell ref="E25:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2046,7 +2136,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2058,7 +2148,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -2073,134 +2163,130 @@
       <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="E3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="22">
+      <c r="A4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="21">
         <f>C4*D4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="22">
+      <c r="A5" s="17"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="21">
         <f t="shared" ref="E5:E7" si="0">C5*D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="22">
+      <c r="A6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="22">
+      <c r="A7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="37"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F12" s="16"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D9:E11"/>
-    <mergeCell ref="G9:H11"/>
-    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F3:H5"/>
+    <mergeCell ref="F8:H12"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B7">
@@ -2215,6 +2301,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
update app, welcome xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="17720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Transportation</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t xml:space="preserve">Add your new expense </t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -95,14 +98,10 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -135,20 +134,10 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF4285F4"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="2" tint="-0.499984740745262"/>
       <name val="FZLanTingHei-M-GBK"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="Arial"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -159,16 +148,13 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF4285F4"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -180,18 +166,20 @@
       <sz val="12"/>
       <color theme="2" tint="-0.499984740745262"/>
       <name val="FZLanTingHei-M-GBK"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="24"/>
       <color theme="2" tint="-0.749992370372631"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,7 +187,26 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="15">
@@ -329,77 +336,71 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="9" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -585,7 +586,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.0196288713650121"/>
-                  <c:y val="-0.0846666666666668"/>
+                  <c:y val="-0.0846666666666669"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1478,15 +1479,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>40021</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>655265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>16009</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1666089</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>181429</xdr:rowOff>
+      <xdr:rowOff>182325</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1508,33 +1509,33 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>132987</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>71173</xdr:rowOff>
+      <xdr:rowOff>75937</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1079500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>913509</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>183537</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5087938" y="5317861"/>
-          <a:ext cx="2563812" cy="427302"/>
+          <a:off x="5123864" y="5386171"/>
+          <a:ext cx="2355025" cy="412103"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1551,33 +1552,33 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>82826</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>116783</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>13805</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>162893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5905500" y="469900"/>
-          <a:ext cx="2705100" cy="450850"/>
+          <a:off x="5894456" y="503305"/>
+          <a:ext cx="2788479" cy="467142"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1589,33 +1590,33 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>96630</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>213968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>185775</xdr:rowOff>
+      <xdr:colOff>11234</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>33683</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5905500" y="1689100"/>
-          <a:ext cx="2768600" cy="579475"/>
+          <a:off x="5908260" y="1732446"/>
+          <a:ext cx="2772104" cy="585857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1895,8 +1896,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1912,162 +1913,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="13"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13"/>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="24">
         <v>3000</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="13"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
+      <c r="A8" s="23">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="13"/>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15">
+      <c r="A11" s="22">
         <f>A5-A8</f>
         <v>3000</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="13"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="13"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="13"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-    </row>
-    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="12">
         <v>0</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="13">
         <v>0</v>
       </c>
-      <c r="D19" s="6" t="e">
+      <c r="D19" s="14" t="e">
         <f>C19/C23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="12">
         <v>0</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="13">
         <v>0</v>
       </c>
-      <c r="D20" s="6" t="e">
+      <c r="D20" s="14" t="e">
         <f>C20/C23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="12">
         <v>0</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="13">
         <v>0</v>
       </c>
-      <c r="D21" s="7" t="e">
+      <c r="D21" s="15" t="e">
         <f>C21/C23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="12">
         <v>0</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="13">
         <v>0</v>
       </c>
-      <c r="D22" s="7" t="e">
+      <c r="D22" s="15" t="e">
         <f>C22/C23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="13">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="8" t="e">
+      <c r="D23" s="16" t="e">
         <f>SUM(D19:D22)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2076,43 +2077,43 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="9"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="9"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="9"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="2"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="9"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="1"/>
     </row>
   </sheetData>
@@ -2122,6 +2123,7 @@
     <mergeCell ref="C25:D28"/>
     <mergeCell ref="E25:H28"/>
   </mergeCells>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2133,10 +2135,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2147,139 +2149,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5">
+        <v>100</v>
+      </c>
+      <c r="E4" s="8">
         <f>C4*D4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+        <v>300</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="21">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="8">
         <f t="shared" ref="E5:E7" si="0">C5*D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="21">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="21">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="31" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+    </row>
+    <row r="19" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2288,20 +2306,27 @@
     <mergeCell ref="F3:H5"/>
     <mergeCell ref="F8:H12"/>
   </mergeCells>
-  <dataValidations count="3">
+  <phoneticPr fontId="17" type="noConversion"/>
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B7">
       <formula1>"Transportation, Lodging, Food, Entertainment"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D7">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D7">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="please input a positive integer" sqref="C4">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="please input a positive integer" sqref="D4">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
update cell format, width of excel file
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="17720" tabRatio="500"/>
+    <workbookView xWindow="33740" yWindow="460" windowWidth="20740" windowHeight="17720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -341,7 +341,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -367,7 +367,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="9" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1902,6 +1901,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
@@ -1913,12 +1913,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
@@ -1927,12 +1927,12 @@
       <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24">
+      <c r="A5" s="23">
         <v>3000</v>
       </c>
     </row>
@@ -1940,12 +1940,12 @@
       <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
@@ -1954,12 +1954,12 @@
       <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <f>A5-A8</f>
         <v>3000</v>
       </c>
@@ -1980,22 +1980,22 @@
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="16" t="e">
+      <c r="D23" s="15" t="e">
         <f>SUM(D19:D22)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2077,42 +2077,42 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
       <c r="I27" s="2"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
       <c r="I28" s="2"/>
       <c r="J28" s="1"/>
     </row>
@@ -2149,40 +2149,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
@@ -2199,9 +2199,9 @@
         <f>C4*D4</f>
         <v>300</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
@@ -2212,9 +2212,9 @@
         <f t="shared" ref="E5:E7" si="0">C5*D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -2248,46 +2248,46 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="19" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I19" t="s">

</xml_diff>

<commit_message>
* update app.xlsx for column width aligned with the chart * set zoom level to 100%
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33740" yWindow="460" windowWidth="20740" windowHeight="17720" tabRatio="500"/>
+    <workbookView xWindow="11180" yWindow="1160" windowWidth="20740" windowHeight="19260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -1895,7 +1895,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -1904,7 +1904,7 @@
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="6.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
* add gridline * update text and focus
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Transportation</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Taxi</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2141,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2185,7 +2188,9 @@
       <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
update a link and header cell size
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="1160" windowWidth="20740" windowHeight="19260" tabRatio="500"/>
+    <workbookView xWindow="36600" yWindow="580" windowWidth="20740" windowHeight="19260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="App-page1" sheetId="3" r:id="rId1"/>
@@ -1899,7 +1899,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1907,7 +1907,7 @@
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
     <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="6.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
fix excel file style issues
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -1559,8 +1559,8 @@
       <xdr:rowOff>116783</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>13805</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1116069</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>162893</xdr:rowOff>
     </xdr:to>
@@ -1911,7 +1911,7 @@
     <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="6.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2143,7 +2143,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2151,6 +2151,7 @@
     <col min="1" max="1" width="14.5" style="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
enlarge a column width to avoid cutting an image
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/app.xlsx
+++ b/src/main/webapp/WEB-INF/book/app.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -97,9 +97,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -369,8 +370,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="9" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -404,6 +403,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
@@ -1560,7 +1561,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1305945</xdr:colOff>
+      <xdr:colOff>1186133</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>214487</xdr:rowOff>
     </xdr:to>
@@ -1598,7 +1599,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1206695</xdr:colOff>
+      <xdr:colOff>1086883</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>47924</xdr:rowOff>
     </xdr:to>
@@ -1911,17 +1912,16 @@
     <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" customWidth="1"/>
     <col min="7" max="7" width="6.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="8" max="9" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
@@ -1930,12 +1930,12 @@
       <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
+      <c r="A5" s="21">
         <v>3000</v>
       </c>
     </row>
@@ -1943,12 +1943,12 @@
       <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
+      <c r="A8" s="20">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
@@ -1958,12 +1958,12 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="21">
+      <c r="A11" s="19">
         <f>A5-A8</f>
         <v>3000</v>
       </c>
@@ -1984,22 +1984,22 @@
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       <c r="C19" s="13">
         <v>0</v>
       </c>
-      <c r="D19" s="14" t="e">
+      <c r="D19" s="29" t="e">
         <f>C19/C23</f>
         <v>#DIV/0!</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="C20" s="13">
         <v>0</v>
       </c>
-      <c r="D20" s="14" t="e">
+      <c r="D20" s="29" t="e">
         <f>C20/C23</f>
         <v>#DIV/0!</v>
       </c>
@@ -2043,7 +2043,7 @@
       <c r="C21" s="13">
         <v>0</v>
       </c>
-      <c r="D21" s="15" t="e">
+      <c r="D21" s="30" t="e">
         <f>C21/C23</f>
         <v>#DIV/0!</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="C22" s="13">
         <v>0</v>
       </c>
-      <c r="D22" s="15" t="e">
+      <c r="D22" s="30" t="e">
         <f>C22/C23</f>
         <v>#DIV/0!</v>
       </c>
@@ -2072,7 +2072,7 @@
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="15" t="e">
+      <c r="D23" s="30" t="e">
         <f>SUM(D19:D22)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2082,42 +2082,42 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="2"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="7" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="2"/>
       <c r="J28" s="1"/>
     </row>
@@ -2143,52 +2143,52 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.5" style="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -2207,9 +2207,9 @@
         <f>C4*D4</f>
         <v>300</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
@@ -2220,9 +2220,9 @@
         <f t="shared" ref="E5:E7" si="0">C5*D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
@@ -2256,46 +2256,46 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="11" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="19" spans="5:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I19" t="s">

</xml_diff>